<commit_message>
add script that generates new manifest templates; update dockerfile and readme to incorporate new script
</commit_message>
<xml_diff>
--- a/manifest_templates/datasets_manifest.xlsx
+++ b/manifest_templates/datasets_manifest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vchung/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7DE467-307B-7E4A-B3FF-A687929C66C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8433BDF3-F6FE-B143-9A0E-080F75BE809B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="20660" windowHeight="17540" xr2:uid="{CD4E31F0-ADA2-D447-8E73-A4C2A56D4DCF}"/>
+    <workbookView xWindow="340" yWindow="500" windowWidth="20660" windowHeight="17500" xr2:uid="{CD4E31F0-ADA2-D447-8E73-A4C2A56D4DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="manifest" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="standard_terms" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">standard_terms!$A$1:$C$426</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">standard_terms!$A$1:$C$493</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="524">
   <si>
     <t>datasetName</t>
   </si>
@@ -1604,6 +1604,12 @@
   </si>
   <si>
     <t>Urothelial Carcinoma</t>
+  </si>
+  <si>
+    <t>Dog</t>
+  </si>
+  <si>
+    <t>Must use controlled-vocabulary terms</t>
   </si>
 </sst>
 </file>
@@ -1635,12 +1641,18 @@
       <name val="SF Mono"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1655,7 +1667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1669,6 +1681,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2020,16 +2033,16 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -2051,36 +2064,6 @@
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Value is not one of the acceptable values for this column. Please see `standard_terms` tab for more information." prompt="Select value from the dropdown list." xr:uid="{78368132-A3B6-944B-A1D5-8732313737DF}">
-          <x14:formula1>
-            <xm:f>standard_terms!$B$2:$B$193</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Value is not one of the acceptable values for this column. Please see `standard_terms` tab for more information." prompt="Select value from the dropdown list." xr:uid="{91EB45EF-6F6E-4242-8094-D312683E852D}">
-          <x14:formula1>
-            <xm:f>standard_terms!$B$194:$B$205</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Value is not one of the acceptable values for this column. Please see `standard_terms` tab for more information." prompt="Select value from the dropdown list." xr:uid="{65206DC8-A846-5141-81A4-0A4F63D38645}">
-          <x14:formula1>
-            <xm:f>standard_terms!$B$343:$B$492</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Value is not one of the acceptable values for this column. Please see `standard_terms` tab for more information." prompt="Select value from the dropdown list." xr:uid="{6B8A426B-C78F-2C48-9BE9-B8AE475FC8AE}">
-          <x14:formula1>
-            <xm:f>standard_terms!$B$206:$B$342</xm:f>
-          </x14:formula1>
-          <xm:sqref>I2:I1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2088,7 +2071,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F424B9EB-732F-B548-908D-2FCF6390E552}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2164,7 +2149,9 @@
       <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
@@ -2173,7 +2160,9 @@
       <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
@@ -2182,7 +2171,9 @@
       <c r="B9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
@@ -2191,7 +2182,9 @@
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="6" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
@@ -2250,9 +2243,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22616EE1-2275-CB41-A986-1AA97511F3EE}">
-  <dimension ref="A1:C492"/>
+  <dimension ref="A1:C493"/>
   <sheetViews>
-    <sheetView topLeftCell="A314" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4429,7 +4422,7 @@
         <v>4</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>158</v>
+        <v>522</v>
       </c>
       <c r="C198" t="s">
         <v>439</v>
@@ -4440,7 +4433,7 @@
         <v>4</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C199" t="s">
         <v>439</v>
@@ -4451,7 +4444,7 @@
         <v>4</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>409</v>
+        <v>159</v>
       </c>
       <c r="C200" t="s">
         <v>439</v>
@@ -4462,7 +4455,7 @@
         <v>4</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>160</v>
+        <v>409</v>
       </c>
       <c r="C201" t="s">
         <v>439</v>
@@ -4473,7 +4466,7 @@
         <v>4</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C202" t="s">
         <v>439</v>
@@ -4484,7 +4477,7 @@
         <v>4</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="C203" t="s">
         <v>439</v>
@@ -4495,7 +4488,7 @@
         <v>4</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>412</v>
+        <v>147</v>
       </c>
       <c r="C204" t="s">
         <v>439</v>
@@ -4506,15 +4499,18 @@
         <v>4</v>
       </c>
       <c r="B205" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C205" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A206" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B206" s="2" t="s">
         <v>411</v>
-      </c>
-      <c r="C205" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A206" t="s">
-        <v>6</v>
       </c>
       <c r="C206" t="s">
         <v>439</v>
@@ -4524,9 +4520,6 @@
       <c r="A207" t="s">
         <v>6</v>
       </c>
-      <c r="B207" t="s">
-        <v>360</v>
-      </c>
       <c r="C207" t="s">
         <v>439</v>
       </c>
@@ -4536,7 +4529,7 @@
         <v>6</v>
       </c>
       <c r="B208" t="s">
-        <v>303</v>
+        <v>360</v>
       </c>
       <c r="C208" t="s">
         <v>439</v>
@@ -4547,7 +4540,7 @@
         <v>6</v>
       </c>
       <c r="B209" t="s">
-        <v>382</v>
+        <v>303</v>
       </c>
       <c r="C209" t="s">
         <v>439</v>
@@ -4558,7 +4551,7 @@
         <v>6</v>
       </c>
       <c r="B210" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C210" t="s">
         <v>439</v>
@@ -4569,7 +4562,7 @@
         <v>6</v>
       </c>
       <c r="B211" t="s">
-        <v>333</v>
+        <v>381</v>
       </c>
       <c r="C211" t="s">
         <v>439</v>
@@ -4580,7 +4573,7 @@
         <v>6</v>
       </c>
       <c r="B212" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C212" t="s">
         <v>439</v>
@@ -4591,7 +4584,7 @@
         <v>6</v>
       </c>
       <c r="B213" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="C213" t="s">
         <v>439</v>
@@ -4602,7 +4595,7 @@
         <v>6</v>
       </c>
       <c r="B214" t="s">
-        <v>387</v>
+        <v>329</v>
       </c>
       <c r="C214" t="s">
         <v>439</v>
@@ -4613,7 +4606,7 @@
         <v>6</v>
       </c>
       <c r="B215" t="s">
-        <v>422</v>
+        <v>387</v>
       </c>
       <c r="C215" t="s">
         <v>439</v>
@@ -4624,7 +4617,7 @@
         <v>6</v>
       </c>
       <c r="B216" t="s">
-        <v>317</v>
+        <v>422</v>
       </c>
       <c r="C216" t="s">
         <v>439</v>
@@ -4635,7 +4628,7 @@
         <v>6</v>
       </c>
       <c r="B217" t="s">
-        <v>351</v>
+        <v>317</v>
       </c>
       <c r="C217" t="s">
         <v>439</v>
@@ -4646,7 +4639,7 @@
         <v>6</v>
       </c>
       <c r="B218" t="s">
-        <v>368</v>
+        <v>351</v>
       </c>
       <c r="C218" t="s">
         <v>439</v>
@@ -4657,7 +4650,7 @@
         <v>6</v>
       </c>
       <c r="B219" t="s">
-        <v>395</v>
+        <v>368</v>
       </c>
       <c r="C219" t="s">
         <v>439</v>
@@ -4668,7 +4661,7 @@
         <v>6</v>
       </c>
       <c r="B220" t="s">
-        <v>318</v>
+        <v>395</v>
       </c>
       <c r="C220" t="s">
         <v>439</v>
@@ -4679,7 +4672,7 @@
         <v>6</v>
       </c>
       <c r="B221" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="C221" t="s">
         <v>439</v>
@@ -4690,7 +4683,7 @@
         <v>6</v>
       </c>
       <c r="B222" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="C222" t="s">
         <v>439</v>
@@ -4701,7 +4694,7 @@
         <v>6</v>
       </c>
       <c r="B223" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="C223" t="s">
         <v>439</v>
@@ -4712,7 +4705,7 @@
         <v>6</v>
       </c>
       <c r="B224" t="s">
-        <v>366</v>
+        <v>322</v>
       </c>
       <c r="C224" t="s">
         <v>439</v>
@@ -4723,7 +4716,7 @@
         <v>6</v>
       </c>
       <c r="B225" t="s">
-        <v>300</v>
+        <v>366</v>
       </c>
       <c r="C225" t="s">
         <v>439</v>
@@ -4734,7 +4727,7 @@
         <v>6</v>
       </c>
       <c r="B226" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="C226" t="s">
         <v>439</v>
@@ -4745,7 +4738,7 @@
         <v>6</v>
       </c>
       <c r="B227" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="C227" t="s">
         <v>439</v>
@@ -4756,7 +4749,7 @@
         <v>6</v>
       </c>
       <c r="B228" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="C228" t="s">
         <v>439</v>
@@ -4767,7 +4760,7 @@
         <v>6</v>
       </c>
       <c r="B229" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="C229" t="s">
         <v>439</v>
@@ -4778,7 +4771,7 @@
         <v>6</v>
       </c>
       <c r="B230" t="s">
-        <v>358</v>
+        <v>308</v>
       </c>
       <c r="C230" t="s">
         <v>439</v>
@@ -4789,7 +4782,7 @@
         <v>6</v>
       </c>
       <c r="B231" t="s">
-        <v>396</v>
+        <v>358</v>
       </c>
       <c r="C231" t="s">
         <v>439</v>
@@ -4800,7 +4793,7 @@
         <v>6</v>
       </c>
       <c r="B232" t="s">
-        <v>383</v>
+        <v>396</v>
       </c>
       <c r="C232" t="s">
         <v>439</v>
@@ -4811,7 +4804,7 @@
         <v>6</v>
       </c>
       <c r="B233" t="s">
-        <v>331</v>
+        <v>383</v>
       </c>
       <c r="C233" t="s">
         <v>439</v>
@@ -4822,7 +4815,7 @@
         <v>6</v>
       </c>
       <c r="B234" t="s">
-        <v>394</v>
+        <v>331</v>
       </c>
       <c r="C234" t="s">
         <v>439</v>
@@ -4833,7 +4826,7 @@
         <v>6</v>
       </c>
       <c r="B235" t="s">
-        <v>304</v>
+        <v>394</v>
       </c>
       <c r="C235" t="s">
         <v>439</v>
@@ -4844,7 +4837,7 @@
         <v>6</v>
       </c>
       <c r="B236" t="s">
-        <v>404</v>
+        <v>304</v>
       </c>
       <c r="C236" t="s">
         <v>439</v>
@@ -4855,7 +4848,7 @@
         <v>6</v>
       </c>
       <c r="B237" t="s">
-        <v>338</v>
+        <v>404</v>
       </c>
       <c r="C237" t="s">
         <v>439</v>
@@ -4866,7 +4859,7 @@
         <v>6</v>
       </c>
       <c r="B238" t="s">
-        <v>375</v>
+        <v>338</v>
       </c>
       <c r="C238" t="s">
         <v>439</v>
@@ -4877,7 +4870,7 @@
         <v>6</v>
       </c>
       <c r="B239" t="s">
-        <v>406</v>
+        <v>375</v>
       </c>
       <c r="C239" t="s">
         <v>439</v>
@@ -4888,7 +4881,7 @@
         <v>6</v>
       </c>
       <c r="B240" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C240" t="s">
         <v>439</v>
@@ -4899,7 +4892,7 @@
         <v>6</v>
       </c>
       <c r="B241" t="s">
-        <v>397</v>
+        <v>405</v>
       </c>
       <c r="C241" t="s">
         <v>439</v>
@@ -4910,7 +4903,7 @@
         <v>6</v>
       </c>
       <c r="B242" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="C242" t="s">
         <v>439</v>
@@ -4921,7 +4914,7 @@
         <v>6</v>
       </c>
       <c r="B243" t="s">
-        <v>357</v>
+        <v>408</v>
       </c>
       <c r="C243" t="s">
         <v>439</v>
@@ -4932,7 +4925,7 @@
         <v>6</v>
       </c>
       <c r="B244" t="s">
-        <v>398</v>
+        <v>357</v>
       </c>
       <c r="C244" t="s">
         <v>439</v>
@@ -4943,7 +4936,7 @@
         <v>6</v>
       </c>
       <c r="B245" t="s">
-        <v>292</v>
+        <v>398</v>
       </c>
       <c r="C245" t="s">
         <v>439</v>
@@ -4954,7 +4947,7 @@
         <v>6</v>
       </c>
       <c r="B246" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C246" t="s">
         <v>439</v>
@@ -4965,7 +4958,7 @@
         <v>6</v>
       </c>
       <c r="B247" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C247" t="s">
         <v>439</v>
@@ -4976,7 +4969,7 @@
         <v>6</v>
       </c>
       <c r="B248" t="s">
-        <v>460</v>
+        <v>291</v>
       </c>
       <c r="C248" t="s">
         <v>439</v>
@@ -4987,7 +4980,7 @@
         <v>6</v>
       </c>
       <c r="B249" t="s">
-        <v>316</v>
+        <v>460</v>
       </c>
       <c r="C249" t="s">
         <v>439</v>
@@ -4998,7 +4991,7 @@
         <v>6</v>
       </c>
       <c r="B250" t="s">
-        <v>367</v>
+        <v>316</v>
       </c>
       <c r="C250" t="s">
         <v>439</v>
@@ -5009,7 +5002,7 @@
         <v>6</v>
       </c>
       <c r="B251" t="s">
-        <v>388</v>
+        <v>367</v>
       </c>
       <c r="C251" t="s">
         <v>439</v>
@@ -5020,7 +5013,7 @@
         <v>6</v>
       </c>
       <c r="B252" t="s">
-        <v>369</v>
+        <v>388</v>
       </c>
       <c r="C252" t="s">
         <v>439</v>
@@ -5031,7 +5024,7 @@
         <v>6</v>
       </c>
       <c r="B253" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C253" t="s">
         <v>439</v>
@@ -5042,7 +5035,7 @@
         <v>6</v>
       </c>
       <c r="B254" t="s">
-        <v>289</v>
+        <v>372</v>
       </c>
       <c r="C254" t="s">
         <v>439</v>
@@ -5053,7 +5046,7 @@
         <v>6</v>
       </c>
       <c r="B255" t="s">
-        <v>350</v>
+        <v>289</v>
       </c>
       <c r="C255" t="s">
         <v>439</v>
@@ -5064,7 +5057,7 @@
         <v>6</v>
       </c>
       <c r="B256" t="s">
-        <v>321</v>
+        <v>350</v>
       </c>
       <c r="C256" t="s">
         <v>439</v>
@@ -5075,7 +5068,7 @@
         <v>6</v>
       </c>
       <c r="B257" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="C257" t="s">
         <v>439</v>
@@ -5086,7 +5079,7 @@
         <v>6</v>
       </c>
       <c r="B258" t="s">
-        <v>377</v>
+        <v>335</v>
       </c>
       <c r="C258" t="s">
         <v>439</v>
@@ -5097,7 +5090,7 @@
         <v>6</v>
       </c>
       <c r="B259" t="s">
-        <v>283</v>
+        <v>377</v>
       </c>
       <c r="C259" t="s">
         <v>439</v>
@@ -5108,7 +5101,7 @@
         <v>6</v>
       </c>
       <c r="B260" t="s">
-        <v>386</v>
+        <v>283</v>
       </c>
       <c r="C260" t="s">
         <v>439</v>
@@ -5119,7 +5112,7 @@
         <v>6</v>
       </c>
       <c r="B261" t="s">
-        <v>282</v>
+        <v>386</v>
       </c>
       <c r="C261" t="s">
         <v>439</v>
@@ -5130,7 +5123,7 @@
         <v>6</v>
       </c>
       <c r="B262" t="s">
-        <v>354</v>
+        <v>282</v>
       </c>
       <c r="C262" t="s">
         <v>439</v>
@@ -5141,7 +5134,7 @@
         <v>6</v>
       </c>
       <c r="B263" t="s">
-        <v>376</v>
+        <v>354</v>
       </c>
       <c r="C263" t="s">
         <v>439</v>
@@ -5152,7 +5145,7 @@
         <v>6</v>
       </c>
       <c r="B264" t="s">
-        <v>287</v>
+        <v>376</v>
       </c>
       <c r="C264" t="s">
         <v>439</v>
@@ -5163,7 +5156,7 @@
         <v>6</v>
       </c>
       <c r="B265" t="s">
-        <v>371</v>
+        <v>287</v>
       </c>
       <c r="C265" t="s">
         <v>439</v>
@@ -5174,7 +5167,7 @@
         <v>6</v>
       </c>
       <c r="B266" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="C266" t="s">
         <v>439</v>
@@ -5185,7 +5178,7 @@
         <v>6</v>
       </c>
       <c r="B267" t="s">
-        <v>345</v>
+        <v>385</v>
       </c>
       <c r="C267" t="s">
         <v>439</v>
@@ -5196,7 +5189,7 @@
         <v>6</v>
       </c>
       <c r="B268" t="s">
-        <v>363</v>
+        <v>345</v>
       </c>
       <c r="C268" t="s">
         <v>439</v>
@@ -5207,7 +5200,7 @@
         <v>6</v>
       </c>
       <c r="B269" t="s">
-        <v>326</v>
+        <v>363</v>
       </c>
       <c r="C269" t="s">
         <v>439</v>
@@ -5218,7 +5211,7 @@
         <v>6</v>
       </c>
       <c r="B270" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C270" t="s">
         <v>439</v>
@@ -5229,7 +5222,7 @@
         <v>6</v>
       </c>
       <c r="B271" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="C271" t="s">
         <v>439</v>
@@ -5240,7 +5233,7 @@
         <v>6</v>
       </c>
       <c r="B272" t="s">
-        <v>279</v>
+        <v>341</v>
       </c>
       <c r="C272" t="s">
         <v>439</v>
@@ -5251,7 +5244,7 @@
         <v>6</v>
       </c>
       <c r="B273" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C273" t="s">
         <v>439</v>
@@ -5262,7 +5255,7 @@
         <v>6</v>
       </c>
       <c r="B274" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="C274" t="s">
         <v>439</v>
@@ -5273,7 +5266,7 @@
         <v>6</v>
       </c>
       <c r="B275" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C275" t="s">
         <v>439</v>
@@ -5284,7 +5277,7 @@
         <v>6</v>
       </c>
       <c r="B276" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="C276" t="s">
         <v>439</v>
@@ -5295,7 +5288,7 @@
         <v>6</v>
       </c>
       <c r="B277" t="s">
-        <v>342</v>
+        <v>280</v>
       </c>
       <c r="C277" t="s">
         <v>439</v>
@@ -5306,7 +5299,7 @@
         <v>6</v>
       </c>
       <c r="B278" t="s">
-        <v>407</v>
+        <v>342</v>
       </c>
       <c r="C278" t="s">
         <v>439</v>
@@ -5317,7 +5310,7 @@
         <v>6</v>
       </c>
       <c r="B279" t="s">
-        <v>378</v>
+        <v>407</v>
       </c>
       <c r="C279" t="s">
         <v>439</v>
@@ -5328,7 +5321,7 @@
         <v>6</v>
       </c>
       <c r="B280" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="C280" t="s">
         <v>439</v>
@@ -5339,7 +5332,7 @@
         <v>6</v>
       </c>
       <c r="B281" t="s">
-        <v>344</v>
+        <v>390</v>
       </c>
       <c r="C281" t="s">
         <v>439</v>
@@ -5350,7 +5343,7 @@
         <v>6</v>
       </c>
       <c r="B282" t="s">
-        <v>362</v>
+        <v>344</v>
       </c>
       <c r="C282" t="s">
         <v>439</v>
@@ -5361,7 +5354,7 @@
         <v>6</v>
       </c>
       <c r="B283" t="s">
-        <v>392</v>
+        <v>362</v>
       </c>
       <c r="C283" t="s">
         <v>439</v>
@@ -5372,7 +5365,7 @@
         <v>6</v>
       </c>
       <c r="B284" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C284" t="s">
         <v>439</v>
@@ -5383,7 +5376,7 @@
         <v>6</v>
       </c>
       <c r="B285" t="s">
-        <v>298</v>
+        <v>389</v>
       </c>
       <c r="C285" t="s">
         <v>439</v>
@@ -5394,7 +5387,7 @@
         <v>6</v>
       </c>
       <c r="B286" t="s">
-        <v>323</v>
+        <v>298</v>
       </c>
       <c r="C286" t="s">
         <v>439</v>
@@ -5405,7 +5398,7 @@
         <v>6</v>
       </c>
       <c r="B287" t="s">
-        <v>311</v>
+        <v>323</v>
       </c>
       <c r="C287" t="s">
         <v>439</v>
@@ -5416,7 +5409,7 @@
         <v>6</v>
       </c>
       <c r="B288" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="C288" t="s">
         <v>439</v>
@@ -5427,7 +5420,7 @@
         <v>6</v>
       </c>
       <c r="B289" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C289" t="s">
         <v>439</v>
@@ -5438,7 +5431,7 @@
         <v>6</v>
       </c>
       <c r="B290" t="s">
-        <v>356</v>
+        <v>302</v>
       </c>
       <c r="C290" t="s">
         <v>439</v>
@@ -5449,7 +5442,7 @@
         <v>6</v>
       </c>
       <c r="B291" t="s">
-        <v>315</v>
+        <v>356</v>
       </c>
       <c r="C291" t="s">
         <v>439</v>
@@ -5460,7 +5453,7 @@
         <v>6</v>
       </c>
       <c r="B292" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="C292" t="s">
         <v>439</v>
@@ -5471,7 +5464,7 @@
         <v>6</v>
       </c>
       <c r="B293" t="s">
-        <v>330</v>
+        <v>305</v>
       </c>
       <c r="C293" t="s">
         <v>439</v>
@@ -5482,7 +5475,7 @@
         <v>6</v>
       </c>
       <c r="B294" t="s">
-        <v>399</v>
+        <v>330</v>
       </c>
       <c r="C294" t="s">
         <v>439</v>
@@ -5493,7 +5486,7 @@
         <v>6</v>
       </c>
       <c r="B295" t="s">
-        <v>340</v>
+        <v>399</v>
       </c>
       <c r="C295" t="s">
         <v>439</v>
@@ -5504,7 +5497,7 @@
         <v>6</v>
       </c>
       <c r="B296" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="C296" t="s">
         <v>439</v>
@@ -5515,7 +5508,7 @@
         <v>6</v>
       </c>
       <c r="B297" t="s">
-        <v>346</v>
+        <v>364</v>
       </c>
       <c r="C297" t="s">
         <v>439</v>
@@ -5526,7 +5519,7 @@
         <v>6</v>
       </c>
       <c r="B298" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="C298" t="s">
         <v>439</v>
@@ -5537,7 +5530,7 @@
         <v>6</v>
       </c>
       <c r="B299" t="s">
-        <v>384</v>
+        <v>355</v>
       </c>
       <c r="C299" t="s">
         <v>439</v>
@@ -5548,7 +5541,7 @@
         <v>6</v>
       </c>
       <c r="B300" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="C300" t="s">
         <v>439</v>
@@ -5559,7 +5552,7 @@
         <v>6</v>
       </c>
       <c r="B301" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="C301" t="s">
         <v>439</v>
@@ -5570,7 +5563,7 @@
         <v>6</v>
       </c>
       <c r="B302" t="s">
-        <v>503</v>
+        <v>373</v>
       </c>
       <c r="C302" t="s">
         <v>439</v>
@@ -5581,7 +5574,7 @@
         <v>6</v>
       </c>
       <c r="B303" t="s">
-        <v>349</v>
+        <v>503</v>
       </c>
       <c r="C303" t="s">
         <v>439</v>
@@ -5592,7 +5585,7 @@
         <v>6</v>
       </c>
       <c r="B304" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C304" t="s">
         <v>439</v>
@@ -5603,7 +5596,7 @@
         <v>6</v>
       </c>
       <c r="B305" t="s">
-        <v>310</v>
+        <v>353</v>
       </c>
       <c r="C305" t="s">
         <v>439</v>
@@ -5614,7 +5607,7 @@
         <v>6</v>
       </c>
       <c r="B306" t="s">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="C306" t="s">
         <v>439</v>
@@ -5625,7 +5618,7 @@
         <v>6</v>
       </c>
       <c r="B307" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="C307" t="s">
         <v>439</v>
@@ -5636,7 +5629,7 @@
         <v>6</v>
       </c>
       <c r="B308" t="s">
-        <v>504</v>
+        <v>306</v>
       </c>
       <c r="C308" t="s">
         <v>439</v>
@@ -5647,7 +5640,7 @@
         <v>6</v>
       </c>
       <c r="B309" t="s">
-        <v>348</v>
+        <v>504</v>
       </c>
       <c r="C309" t="s">
         <v>439</v>
@@ -5658,7 +5651,7 @@
         <v>6</v>
       </c>
       <c r="B310" t="s">
-        <v>370</v>
+        <v>348</v>
       </c>
       <c r="C310" t="s">
         <v>439</v>
@@ -5669,7 +5662,7 @@
         <v>6</v>
       </c>
       <c r="B311" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C311" t="s">
         <v>439</v>
@@ -5680,7 +5673,7 @@
         <v>6</v>
       </c>
       <c r="B312" t="s">
-        <v>320</v>
+        <v>380</v>
       </c>
       <c r="C312" t="s">
         <v>439</v>
@@ -5691,7 +5684,7 @@
         <v>6</v>
       </c>
       <c r="B313" t="s">
-        <v>339</v>
+        <v>320</v>
       </c>
       <c r="C313" t="s">
         <v>439</v>
@@ -5702,7 +5695,7 @@
         <v>6</v>
       </c>
       <c r="B314" t="s">
-        <v>288</v>
+        <v>339</v>
       </c>
       <c r="C314" t="s">
         <v>439</v>
@@ -5713,7 +5706,7 @@
         <v>6</v>
       </c>
       <c r="B315" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="C315" t="s">
         <v>439</v>
@@ -5724,7 +5717,7 @@
         <v>6</v>
       </c>
       <c r="B316" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C316" t="s">
         <v>439</v>
@@ -5735,7 +5728,7 @@
         <v>6</v>
       </c>
       <c r="B317" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="C317" t="s">
         <v>439</v>
@@ -5746,7 +5739,7 @@
         <v>6</v>
       </c>
       <c r="B318" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C318" t="s">
         <v>439</v>
@@ -5757,7 +5750,7 @@
         <v>6</v>
       </c>
       <c r="B319" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C319" t="s">
         <v>439</v>
@@ -5768,7 +5761,7 @@
         <v>6</v>
       </c>
       <c r="B320" t="s">
-        <v>374</v>
+        <v>295</v>
       </c>
       <c r="C320" t="s">
         <v>439</v>
@@ -5779,7 +5772,7 @@
         <v>6</v>
       </c>
       <c r="B321" t="s">
-        <v>299</v>
+        <v>374</v>
       </c>
       <c r="C321" t="s">
         <v>439</v>
@@ -5790,7 +5783,7 @@
         <v>6</v>
       </c>
       <c r="B322" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="C322" t="s">
         <v>439</v>
@@ -5801,7 +5794,7 @@
         <v>6</v>
       </c>
       <c r="B323" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="C323" t="s">
         <v>439</v>
@@ -5812,7 +5805,7 @@
         <v>6</v>
       </c>
       <c r="B324" t="s">
-        <v>365</v>
+        <v>337</v>
       </c>
       <c r="C324" t="s">
         <v>439</v>
@@ -5823,7 +5816,7 @@
         <v>6</v>
       </c>
       <c r="B325" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="C325" t="s">
         <v>439</v>
@@ -5834,7 +5827,7 @@
         <v>6</v>
       </c>
       <c r="B326" t="s">
-        <v>309</v>
+        <v>352</v>
       </c>
       <c r="C326" t="s">
         <v>439</v>
@@ -5845,7 +5838,7 @@
         <v>6</v>
       </c>
       <c r="B327" t="s">
-        <v>402</v>
+        <v>309</v>
       </c>
       <c r="C327" t="s">
         <v>439</v>
@@ -5856,7 +5849,7 @@
         <v>6</v>
       </c>
       <c r="B328" t="s">
-        <v>359</v>
+        <v>402</v>
       </c>
       <c r="C328" t="s">
         <v>439</v>
@@ -5867,7 +5860,7 @@
         <v>6</v>
       </c>
       <c r="B329" t="s">
-        <v>391</v>
+        <v>359</v>
       </c>
       <c r="C329" t="s">
         <v>439</v>
@@ -5878,7 +5871,7 @@
         <v>6</v>
       </c>
       <c r="B330" t="s">
-        <v>423</v>
+        <v>391</v>
       </c>
       <c r="C330" t="s">
         <v>439</v>
@@ -5889,7 +5882,7 @@
         <v>6</v>
       </c>
       <c r="B331" t="s">
-        <v>393</v>
+        <v>423</v>
       </c>
       <c r="C331" t="s">
         <v>439</v>
@@ -5900,7 +5893,7 @@
         <v>6</v>
       </c>
       <c r="B332" t="s">
-        <v>347</v>
+        <v>393</v>
       </c>
       <c r="C332" t="s">
         <v>439</v>
@@ -5911,7 +5904,7 @@
         <v>6</v>
       </c>
       <c r="B333" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
       <c r="C333" t="s">
         <v>439</v>
@@ -5922,7 +5915,7 @@
         <v>6</v>
       </c>
       <c r="B334" t="s">
-        <v>403</v>
+        <v>336</v>
       </c>
       <c r="C334" t="s">
         <v>439</v>
@@ -5933,7 +5926,7 @@
         <v>6</v>
       </c>
       <c r="B335" t="s">
-        <v>147</v>
+        <v>403</v>
       </c>
       <c r="C335" t="s">
         <v>439</v>
@@ -5944,7 +5937,7 @@
         <v>6</v>
       </c>
       <c r="B336" t="s">
-        <v>343</v>
+        <v>147</v>
       </c>
       <c r="C336" t="s">
         <v>439</v>
@@ -5955,7 +5948,7 @@
         <v>6</v>
       </c>
       <c r="B337" t="s">
-        <v>361</v>
+        <v>343</v>
       </c>
       <c r="C337" t="s">
         <v>439</v>
@@ -5966,7 +5959,7 @@
         <v>6</v>
       </c>
       <c r="B338" t="s">
-        <v>325</v>
+        <v>361</v>
       </c>
       <c r="C338" t="s">
         <v>439</v>
@@ -5977,7 +5970,7 @@
         <v>6</v>
       </c>
       <c r="B339" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C339" t="s">
         <v>439</v>
@@ -5988,7 +5981,7 @@
         <v>6</v>
       </c>
       <c r="B340" t="s">
-        <v>401</v>
+        <v>327</v>
       </c>
       <c r="C340" t="s">
         <v>439</v>
@@ -5999,7 +5992,7 @@
         <v>6</v>
       </c>
       <c r="B341" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C341" t="s">
         <v>439</v>
@@ -6010,28 +6003,28 @@
         <v>6</v>
       </c>
       <c r="B342" t="s">
+        <v>400</v>
+      </c>
+      <c r="C342" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A343" t="s">
+        <v>6</v>
+      </c>
+      <c r="B343" t="s">
         <v>312</v>
       </c>
-      <c r="C342" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A343" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B343" s="2"/>
       <c r="C343" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A344" t="s">
-        <v>5</v>
-      </c>
-      <c r="B344" t="s">
-        <v>103</v>
-      </c>
+      <c r="A344" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B344" s="2"/>
       <c r="C344" t="s">
         <v>439</v>
       </c>
@@ -6041,7 +6034,7 @@
         <v>5</v>
       </c>
       <c r="B345" t="s">
-        <v>162</v>
+        <v>103</v>
       </c>
       <c r="C345" t="s">
         <v>439</v>
@@ -6052,7 +6045,7 @@
         <v>5</v>
       </c>
       <c r="B346" t="s">
-        <v>258</v>
+        <v>162</v>
       </c>
       <c r="C346" t="s">
         <v>439</v>
@@ -6063,7 +6056,7 @@
         <v>5</v>
       </c>
       <c r="B347" t="s">
-        <v>203</v>
+        <v>258</v>
       </c>
       <c r="C347" t="s">
         <v>439</v>
@@ -6074,7 +6067,7 @@
         <v>5</v>
       </c>
       <c r="B348" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="C348" t="s">
         <v>439</v>
@@ -6085,7 +6078,7 @@
         <v>5</v>
       </c>
       <c r="B349" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C349" t="s">
         <v>439</v>
@@ -6096,7 +6089,7 @@
         <v>5</v>
       </c>
       <c r="B350" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C350" t="s">
         <v>439</v>
@@ -6107,7 +6100,7 @@
         <v>5</v>
       </c>
       <c r="B351" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="C351" t="s">
         <v>439</v>
@@ -6118,7 +6111,7 @@
         <v>5</v>
       </c>
       <c r="B352" t="s">
-        <v>505</v>
+        <v>204</v>
       </c>
       <c r="C352" t="s">
         <v>439</v>
@@ -6129,7 +6122,7 @@
         <v>5</v>
       </c>
       <c r="B353" t="s">
-        <v>252</v>
+        <v>505</v>
       </c>
       <c r="C353" t="s">
         <v>439</v>
@@ -6140,7 +6133,7 @@
         <v>5</v>
       </c>
       <c r="B354" t="s">
-        <v>225</v>
+        <v>252</v>
       </c>
       <c r="C354" t="s">
         <v>439</v>
@@ -6151,7 +6144,7 @@
         <v>5</v>
       </c>
       <c r="B355" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="C355" t="s">
         <v>439</v>
@@ -6162,7 +6155,7 @@
         <v>5</v>
       </c>
       <c r="B356" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="C356" t="s">
         <v>439</v>
@@ -6173,7 +6166,7 @@
         <v>5</v>
       </c>
       <c r="B357" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="C357" t="s">
         <v>439</v>
@@ -6184,7 +6177,7 @@
         <v>5</v>
       </c>
       <c r="B358" t="s">
-        <v>506</v>
+        <v>163</v>
       </c>
       <c r="C358" t="s">
         <v>439</v>
@@ -6195,7 +6188,7 @@
         <v>5</v>
       </c>
       <c r="B359" t="s">
-        <v>165</v>
+        <v>506</v>
       </c>
       <c r="C359" t="s">
         <v>439</v>
@@ -6206,7 +6199,7 @@
         <v>5</v>
       </c>
       <c r="B360" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C360" t="s">
         <v>439</v>
@@ -6217,7 +6210,7 @@
         <v>5</v>
       </c>
       <c r="B361" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C361" t="s">
         <v>439</v>
@@ -6228,7 +6221,7 @@
         <v>5</v>
       </c>
       <c r="B362" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C362" t="s">
         <v>439</v>
@@ -6239,7 +6232,7 @@
         <v>5</v>
       </c>
       <c r="B363" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C363" t="s">
         <v>439</v>
@@ -6250,7 +6243,7 @@
         <v>5</v>
       </c>
       <c r="B364" t="s">
-        <v>442</v>
+        <v>173</v>
       </c>
       <c r="C364" t="s">
         <v>439</v>
@@ -6261,7 +6254,7 @@
         <v>5</v>
       </c>
       <c r="B365" t="s">
-        <v>179</v>
+        <v>442</v>
       </c>
       <c r="C365" t="s">
         <v>439</v>
@@ -6272,7 +6265,7 @@
         <v>5</v>
       </c>
       <c r="B366" t="s">
-        <v>226</v>
+        <v>179</v>
       </c>
       <c r="C366" t="s">
         <v>439</v>
@@ -6283,7 +6276,7 @@
         <v>5</v>
       </c>
       <c r="B367" t="s">
-        <v>507</v>
+        <v>226</v>
       </c>
       <c r="C367" t="s">
         <v>439</v>
@@ -6294,7 +6287,7 @@
         <v>5</v>
       </c>
       <c r="B368" t="s">
-        <v>206</v>
+        <v>507</v>
       </c>
       <c r="C368" t="s">
         <v>439</v>
@@ -6305,7 +6298,7 @@
         <v>5</v>
       </c>
       <c r="B369" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C369" t="s">
         <v>439</v>
@@ -6316,7 +6309,7 @@
         <v>5</v>
       </c>
       <c r="B370" t="s">
-        <v>167</v>
+        <v>207</v>
       </c>
       <c r="C370" t="s">
         <v>439</v>
@@ -6327,7 +6320,7 @@
         <v>5</v>
       </c>
       <c r="B371" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="C371" t="s">
         <v>439</v>
@@ -6338,7 +6331,7 @@
         <v>5</v>
       </c>
       <c r="B372" t="s">
-        <v>247</v>
+        <v>180</v>
       </c>
       <c r="C372" t="s">
         <v>439</v>
@@ -6349,7 +6342,7 @@
         <v>5</v>
       </c>
       <c r="B373" t="s">
-        <v>189</v>
+        <v>247</v>
       </c>
       <c r="C373" t="s">
         <v>439</v>
@@ -6360,7 +6353,7 @@
         <v>5</v>
       </c>
       <c r="B374" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C374" t="s">
         <v>439</v>
@@ -6371,7 +6364,7 @@
         <v>5</v>
       </c>
       <c r="B375" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="C375" t="s">
         <v>439</v>
@@ -6382,7 +6375,7 @@
         <v>5</v>
       </c>
       <c r="B376" t="s">
-        <v>268</v>
+        <v>211</v>
       </c>
       <c r="C376" t="s">
         <v>439</v>
@@ -6393,7 +6386,7 @@
         <v>5</v>
       </c>
       <c r="B377" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C377" t="s">
         <v>439</v>
@@ -6404,7 +6397,7 @@
         <v>5</v>
       </c>
       <c r="B378" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="C378" t="s">
         <v>439</v>
@@ -6415,7 +6408,7 @@
         <v>5</v>
       </c>
       <c r="B379" t="s">
-        <v>174</v>
+        <v>253</v>
       </c>
       <c r="C379" t="s">
         <v>439</v>
@@ -6426,7 +6419,7 @@
         <v>5</v>
       </c>
       <c r="B380" t="s">
-        <v>508</v>
+        <v>174</v>
       </c>
       <c r="C380" t="s">
         <v>439</v>
@@ -6437,7 +6430,7 @@
         <v>5</v>
       </c>
       <c r="B381" t="s">
-        <v>190</v>
+        <v>508</v>
       </c>
       <c r="C381" t="s">
         <v>439</v>
@@ -6448,7 +6441,7 @@
         <v>5</v>
       </c>
       <c r="B382" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
       <c r="C382" t="s">
         <v>439</v>
@@ -6459,7 +6452,7 @@
         <v>5</v>
       </c>
       <c r="B383" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C383" t="s">
         <v>439</v>
@@ -6470,7 +6463,7 @@
         <v>5</v>
       </c>
       <c r="B384" t="s">
-        <v>197</v>
+        <v>164</v>
       </c>
       <c r="C384" t="s">
         <v>439</v>
@@ -6481,7 +6474,7 @@
         <v>5</v>
       </c>
       <c r="B385" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="C385" t="s">
         <v>439</v>
@@ -6492,7 +6485,7 @@
         <v>5</v>
       </c>
       <c r="B386" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C386" t="s">
         <v>439</v>
@@ -6503,7 +6496,7 @@
         <v>5</v>
       </c>
       <c r="B387" t="s">
-        <v>425</v>
+        <v>228</v>
       </c>
       <c r="C387" t="s">
         <v>439</v>
@@ -6514,7 +6507,7 @@
         <v>5</v>
       </c>
       <c r="B388" t="s">
-        <v>193</v>
+        <v>425</v>
       </c>
       <c r="C388" t="s">
         <v>439</v>
@@ -6525,7 +6518,7 @@
         <v>5</v>
       </c>
       <c r="B389" t="s">
-        <v>461</v>
+        <v>193</v>
       </c>
       <c r="C389" t="s">
         <v>439</v>
@@ -6536,7 +6529,7 @@
         <v>5</v>
       </c>
       <c r="B390" t="s">
-        <v>194</v>
+        <v>461</v>
       </c>
       <c r="C390" t="s">
         <v>439</v>
@@ -6547,7 +6540,7 @@
         <v>5</v>
       </c>
       <c r="B391" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C391" t="s">
         <v>439</v>
@@ -6558,7 +6551,7 @@
         <v>5</v>
       </c>
       <c r="B392" t="s">
-        <v>462</v>
+        <v>195</v>
       </c>
       <c r="C392" t="s">
         <v>439</v>
@@ -6569,7 +6562,7 @@
         <v>5</v>
       </c>
       <c r="B393" t="s">
-        <v>509</v>
+        <v>462</v>
       </c>
       <c r="C393" t="s">
         <v>439</v>
@@ -6580,7 +6573,7 @@
         <v>5</v>
       </c>
       <c r="B394" t="s">
-        <v>196</v>
+        <v>509</v>
       </c>
       <c r="C394" t="s">
         <v>439</v>
@@ -6591,7 +6584,7 @@
         <v>5</v>
       </c>
       <c r="B395" t="s">
-        <v>229</v>
+        <v>196</v>
       </c>
       <c r="C395" t="s">
         <v>439</v>
@@ -6602,7 +6595,7 @@
         <v>5</v>
       </c>
       <c r="B396" t="s">
-        <v>272</v>
+        <v>229</v>
       </c>
       <c r="C396" t="s">
         <v>439</v>
@@ -6613,7 +6606,7 @@
         <v>5</v>
       </c>
       <c r="B397" t="s">
-        <v>427</v>
+        <v>272</v>
       </c>
       <c r="C397" t="s">
         <v>439</v>
@@ -6624,7 +6617,7 @@
         <v>5</v>
       </c>
       <c r="B398" t="s">
-        <v>278</v>
+        <v>427</v>
       </c>
       <c r="C398" t="s">
         <v>439</v>
@@ -6635,7 +6628,7 @@
         <v>5</v>
       </c>
       <c r="B399" t="s">
-        <v>254</v>
+        <v>278</v>
       </c>
       <c r="C399" t="s">
         <v>439</v>
@@ -6646,7 +6639,7 @@
         <v>5</v>
       </c>
       <c r="B400" t="s">
-        <v>463</v>
+        <v>254</v>
       </c>
       <c r="C400" t="s">
         <v>439</v>
@@ -6657,7 +6650,7 @@
         <v>5</v>
       </c>
       <c r="B401" t="s">
-        <v>510</v>
+        <v>463</v>
       </c>
       <c r="C401" t="s">
         <v>439</v>
@@ -6668,7 +6661,7 @@
         <v>5</v>
       </c>
       <c r="B402" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C402" t="s">
         <v>439</v>
@@ -6679,7 +6672,7 @@
         <v>5</v>
       </c>
       <c r="B403" t="s">
-        <v>424</v>
+        <v>511</v>
       </c>
       <c r="C403" t="s">
         <v>439</v>
@@ -6690,7 +6683,7 @@
         <v>5</v>
       </c>
       <c r="B404" t="s">
-        <v>512</v>
+        <v>424</v>
       </c>
       <c r="C404" t="s">
         <v>439</v>
@@ -6701,7 +6694,7 @@
         <v>5</v>
       </c>
       <c r="B405" t="s">
-        <v>276</v>
+        <v>512</v>
       </c>
       <c r="C405" t="s">
         <v>439</v>
@@ -6712,7 +6705,7 @@
         <v>5</v>
       </c>
       <c r="B406" t="s">
-        <v>175</v>
+        <v>276</v>
       </c>
       <c r="C406" t="s">
         <v>439</v>
@@ -6723,7 +6716,7 @@
         <v>5</v>
       </c>
       <c r="B407" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C407" t="s">
         <v>439</v>
@@ -6734,7 +6727,7 @@
         <v>5</v>
       </c>
       <c r="B408" t="s">
-        <v>214</v>
+        <v>176</v>
       </c>
       <c r="C408" t="s">
         <v>439</v>
@@ -6745,7 +6738,7 @@
         <v>5</v>
       </c>
       <c r="B409" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C409" t="s">
         <v>439</v>
@@ -6756,7 +6749,7 @@
         <v>5</v>
       </c>
       <c r="B410" t="s">
-        <v>441</v>
+        <v>215</v>
       </c>
       <c r="C410" t="s">
         <v>439</v>
@@ -6767,7 +6760,7 @@
         <v>5</v>
       </c>
       <c r="B411" t="s">
-        <v>230</v>
+        <v>441</v>
       </c>
       <c r="C411" t="s">
         <v>439</v>
@@ -6778,7 +6771,7 @@
         <v>5</v>
       </c>
       <c r="B412" t="s">
-        <v>275</v>
+        <v>230</v>
       </c>
       <c r="C412" t="s">
         <v>439</v>
@@ -6789,7 +6782,7 @@
         <v>5</v>
       </c>
       <c r="B413" t="s">
-        <v>181</v>
+        <v>275</v>
       </c>
       <c r="C413" t="s">
         <v>439</v>
@@ -6800,7 +6793,7 @@
         <v>5</v>
       </c>
       <c r="B414" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C414" t="s">
         <v>439</v>
@@ -6811,7 +6804,7 @@
         <v>5</v>
       </c>
       <c r="B415" t="s">
-        <v>231</v>
+        <v>182</v>
       </c>
       <c r="C415" t="s">
         <v>439</v>
@@ -6822,7 +6815,7 @@
         <v>5</v>
       </c>
       <c r="B416" t="s">
-        <v>198</v>
+        <v>231</v>
       </c>
       <c r="C416" t="s">
         <v>439</v>
@@ -6833,7 +6826,7 @@
         <v>5</v>
       </c>
       <c r="B417" t="s">
-        <v>440</v>
+        <v>198</v>
       </c>
       <c r="C417" t="s">
         <v>439</v>
@@ -6844,7 +6837,7 @@
         <v>5</v>
       </c>
       <c r="B418" t="s">
-        <v>245</v>
+        <v>440</v>
       </c>
       <c r="C418" t="s">
         <v>439</v>
@@ -6855,7 +6848,7 @@
         <v>5</v>
       </c>
       <c r="B419" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C419" t="s">
         <v>439</v>
@@ -6866,7 +6859,7 @@
         <v>5</v>
       </c>
       <c r="B420" t="s">
-        <v>183</v>
+        <v>246</v>
       </c>
       <c r="C420" t="s">
         <v>439</v>
@@ -6877,7 +6870,7 @@
         <v>5</v>
       </c>
       <c r="B421" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C421" t="s">
         <v>439</v>
@@ -6888,7 +6881,7 @@
         <v>5</v>
       </c>
       <c r="B422" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C422" t="s">
         <v>439</v>
@@ -6899,7 +6892,7 @@
         <v>5</v>
       </c>
       <c r="B423" t="s">
-        <v>248</v>
+        <v>185</v>
       </c>
       <c r="C423" t="s">
         <v>439</v>
@@ -6910,7 +6903,7 @@
         <v>5</v>
       </c>
       <c r="B424" t="s">
-        <v>464</v>
+        <v>248</v>
       </c>
       <c r="C424" t="s">
         <v>439</v>
@@ -6921,7 +6914,7 @@
         <v>5</v>
       </c>
       <c r="B425" t="s">
-        <v>249</v>
+        <v>464</v>
       </c>
       <c r="C425" t="s">
         <v>439</v>
@@ -6932,7 +6925,7 @@
         <v>5</v>
       </c>
       <c r="B426" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C426" t="s">
         <v>439</v>
@@ -6943,7 +6936,7 @@
         <v>5</v>
       </c>
       <c r="B427" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C427" t="s">
         <v>439</v>
@@ -6954,7 +6947,7 @@
         <v>5</v>
       </c>
       <c r="B428" t="s">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="C428" t="s">
         <v>439</v>
@@ -6965,7 +6958,7 @@
         <v>5</v>
       </c>
       <c r="B429" t="s">
-        <v>426</v>
+        <v>232</v>
       </c>
       <c r="C429" t="s">
         <v>439</v>
@@ -6976,7 +6969,7 @@
         <v>5</v>
       </c>
       <c r="B430" t="s">
-        <v>233</v>
+        <v>426</v>
       </c>
       <c r="C430" t="s">
         <v>439</v>
@@ -6987,7 +6980,7 @@
         <v>5</v>
       </c>
       <c r="B431" t="s">
-        <v>513</v>
+        <v>233</v>
       </c>
       <c r="C431" t="s">
         <v>439</v>
@@ -6998,7 +6991,7 @@
         <v>5</v>
       </c>
       <c r="B432" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C432" t="s">
         <v>439</v>
@@ -7009,7 +7002,7 @@
         <v>5</v>
       </c>
       <c r="B433" t="s">
-        <v>177</v>
+        <v>514</v>
       </c>
       <c r="C433" t="s">
         <v>439</v>
@@ -7020,7 +7013,7 @@
         <v>5</v>
       </c>
       <c r="B434" t="s">
-        <v>259</v>
+        <v>177</v>
       </c>
       <c r="C434" t="s">
         <v>439</v>
@@ -7031,7 +7024,7 @@
         <v>5</v>
       </c>
       <c r="B435" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C435" t="s">
         <v>439</v>
@@ -7042,7 +7035,7 @@
         <v>5</v>
       </c>
       <c r="B436" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="C436" t="s">
         <v>439</v>
@@ -7053,7 +7046,7 @@
         <v>5</v>
       </c>
       <c r="B437" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C437" t="s">
         <v>439</v>
@@ -7064,7 +7057,7 @@
         <v>5</v>
       </c>
       <c r="B438" t="s">
-        <v>234</v>
+        <v>256</v>
       </c>
       <c r="C438" t="s">
         <v>439</v>
@@ -7075,7 +7068,7 @@
         <v>5</v>
       </c>
       <c r="B439" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C439" t="s">
         <v>439</v>
@@ -7086,7 +7079,7 @@
         <v>5</v>
       </c>
       <c r="B440" t="s">
-        <v>178</v>
+        <v>235</v>
       </c>
       <c r="C440" t="s">
         <v>439</v>
@@ -7097,7 +7090,7 @@
         <v>5</v>
       </c>
       <c r="B441" t="s">
-        <v>273</v>
+        <v>178</v>
       </c>
       <c r="C441" t="s">
         <v>439</v>
@@ -7108,7 +7101,7 @@
         <v>5</v>
       </c>
       <c r="B442" t="s">
-        <v>515</v>
+        <v>273</v>
       </c>
       <c r="C442" t="s">
         <v>439</v>
@@ -7119,7 +7112,7 @@
         <v>5</v>
       </c>
       <c r="B443" t="s">
-        <v>236</v>
+        <v>515</v>
       </c>
       <c r="C443" t="s">
         <v>439</v>
@@ -7130,7 +7123,7 @@
         <v>5</v>
       </c>
       <c r="B444" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="C444" t="s">
         <v>439</v>
@@ -7141,7 +7134,7 @@
         <v>5</v>
       </c>
       <c r="B445" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
       <c r="C445" t="s">
         <v>439</v>
@@ -7152,7 +7145,7 @@
         <v>5</v>
       </c>
       <c r="B446" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C446" t="s">
         <v>439</v>
@@ -7163,7 +7156,7 @@
         <v>5</v>
       </c>
       <c r="B447" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C447" t="s">
         <v>439</v>
@@ -7174,7 +7167,7 @@
         <v>5</v>
       </c>
       <c r="B448" t="s">
-        <v>199</v>
+        <v>239</v>
       </c>
       <c r="C448" t="s">
         <v>439</v>
@@ -7185,7 +7178,7 @@
         <v>5</v>
       </c>
       <c r="B449" t="s">
-        <v>257</v>
+        <v>199</v>
       </c>
       <c r="C449" t="s">
         <v>439</v>
@@ -7196,7 +7189,7 @@
         <v>5</v>
       </c>
       <c r="B450" t="s">
-        <v>208</v>
+        <v>257</v>
       </c>
       <c r="C450" t="s">
         <v>439</v>
@@ -7207,7 +7200,7 @@
         <v>5</v>
       </c>
       <c r="B451" t="s">
-        <v>267</v>
+        <v>208</v>
       </c>
       <c r="C451" t="s">
         <v>439</v>
@@ -7218,7 +7211,7 @@
         <v>5</v>
       </c>
       <c r="B452" t="s">
-        <v>516</v>
+        <v>267</v>
       </c>
       <c r="C452" t="s">
         <v>439</v>
@@ -7229,7 +7222,7 @@
         <v>5</v>
       </c>
       <c r="B453" t="s">
-        <v>240</v>
+        <v>516</v>
       </c>
       <c r="C453" t="s">
         <v>439</v>
@@ -7240,7 +7233,7 @@
         <v>5</v>
       </c>
       <c r="B454" t="s">
-        <v>217</v>
+        <v>240</v>
       </c>
       <c r="C454" t="s">
         <v>439</v>
@@ -7251,7 +7244,7 @@
         <v>5</v>
       </c>
       <c r="B455" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C455" t="s">
         <v>439</v>
@@ -7262,7 +7255,7 @@
         <v>5</v>
       </c>
       <c r="B456" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
       <c r="C456" t="s">
         <v>439</v>
@@ -7273,7 +7266,7 @@
         <v>5</v>
       </c>
       <c r="B457" t="s">
-        <v>260</v>
+        <v>200</v>
       </c>
       <c r="C457" t="s">
         <v>439</v>
@@ -7284,7 +7277,7 @@
         <v>5</v>
       </c>
       <c r="B458" t="s">
-        <v>465</v>
+        <v>260</v>
       </c>
       <c r="C458" t="s">
         <v>439</v>
@@ -7295,7 +7288,7 @@
         <v>5</v>
       </c>
       <c r="B459" t="s">
-        <v>262</v>
+        <v>465</v>
       </c>
       <c r="C459" t="s">
         <v>439</v>
@@ -7306,7 +7299,7 @@
         <v>5</v>
       </c>
       <c r="B460" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C460" t="s">
         <v>439</v>
@@ -7317,7 +7310,7 @@
         <v>5</v>
       </c>
       <c r="B461" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C461" t="s">
         <v>439</v>
@@ -7328,7 +7321,7 @@
         <v>5</v>
       </c>
       <c r="B462" t="s">
-        <v>517</v>
+        <v>264</v>
       </c>
       <c r="C462" t="s">
         <v>439</v>
@@ -7339,7 +7332,7 @@
         <v>5</v>
       </c>
       <c r="B463" t="s">
-        <v>466</v>
+        <v>517</v>
       </c>
       <c r="C463" t="s">
         <v>439</v>
@@ -7350,7 +7343,7 @@
         <v>5</v>
       </c>
       <c r="B464" t="s">
-        <v>265</v>
+        <v>466</v>
       </c>
       <c r="C464" t="s">
         <v>439</v>
@@ -7361,7 +7354,7 @@
         <v>5</v>
       </c>
       <c r="B465" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C465" t="s">
         <v>439</v>
@@ -7372,7 +7365,7 @@
         <v>5</v>
       </c>
       <c r="B466" t="s">
-        <v>186</v>
+        <v>266</v>
       </c>
       <c r="C466" t="s">
         <v>439</v>
@@ -7383,7 +7376,7 @@
         <v>5</v>
       </c>
       <c r="B467" t="s">
-        <v>518</v>
+        <v>186</v>
       </c>
       <c r="C467" t="s">
         <v>439</v>
@@ -7394,7 +7387,7 @@
         <v>5</v>
       </c>
       <c r="B468" t="s">
-        <v>220</v>
+        <v>518</v>
       </c>
       <c r="C468" t="s">
         <v>439</v>
@@ -7405,7 +7398,7 @@
         <v>5</v>
       </c>
       <c r="B469" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
       <c r="C469" t="s">
         <v>439</v>
@@ -7416,7 +7409,7 @@
         <v>5</v>
       </c>
       <c r="B470" t="s">
-        <v>519</v>
+        <v>241</v>
       </c>
       <c r="C470" t="s">
         <v>439</v>
@@ -7427,7 +7420,7 @@
         <v>5</v>
       </c>
       <c r="B471" t="s">
-        <v>269</v>
+        <v>519</v>
       </c>
       <c r="C471" t="s">
         <v>439</v>
@@ -7438,7 +7431,7 @@
         <v>5</v>
       </c>
       <c r="B472" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C472" t="s">
         <v>439</v>
@@ -7449,7 +7442,7 @@
         <v>5</v>
       </c>
       <c r="B473" t="s">
-        <v>169</v>
+        <v>270</v>
       </c>
       <c r="C473" t="s">
         <v>439</v>
@@ -7460,7 +7453,7 @@
         <v>5</v>
       </c>
       <c r="B474" t="s">
-        <v>244</v>
+        <v>169</v>
       </c>
       <c r="C474" t="s">
         <v>439</v>
@@ -7471,7 +7464,7 @@
         <v>5</v>
       </c>
       <c r="B475" t="s">
-        <v>202</v>
+        <v>244</v>
       </c>
       <c r="C475" t="s">
         <v>439</v>
@@ -7482,7 +7475,7 @@
         <v>5</v>
       </c>
       <c r="B476" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C476" t="s">
         <v>439</v>
@@ -7493,7 +7486,7 @@
         <v>5</v>
       </c>
       <c r="B477" t="s">
-        <v>467</v>
+        <v>201</v>
       </c>
       <c r="C477" t="s">
         <v>439</v>
@@ -7504,7 +7497,7 @@
         <v>5</v>
       </c>
       <c r="B478" t="s">
-        <v>274</v>
+        <v>467</v>
       </c>
       <c r="C478" t="s">
         <v>439</v>
@@ -7515,7 +7508,7 @@
         <v>5</v>
       </c>
       <c r="B479" t="s">
-        <v>520</v>
+        <v>274</v>
       </c>
       <c r="C479" t="s">
         <v>439</v>
@@ -7526,7 +7519,7 @@
         <v>5</v>
       </c>
       <c r="B480" t="s">
-        <v>221</v>
+        <v>520</v>
       </c>
       <c r="C480" t="s">
         <v>439</v>
@@ -7537,7 +7530,7 @@
         <v>5</v>
       </c>
       <c r="B481" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="C481" t="s">
         <v>439</v>
@@ -7548,7 +7541,7 @@
         <v>5</v>
       </c>
       <c r="B482" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="C482" t="s">
         <v>439</v>
@@ -7559,7 +7552,7 @@
         <v>5</v>
       </c>
       <c r="B483" t="s">
-        <v>277</v>
+        <v>219</v>
       </c>
       <c r="C483" t="s">
         <v>439</v>
@@ -7570,7 +7563,7 @@
         <v>5</v>
       </c>
       <c r="B484" t="s">
-        <v>170</v>
+        <v>277</v>
       </c>
       <c r="C484" t="s">
         <v>439</v>
@@ -7581,7 +7574,7 @@
         <v>5</v>
       </c>
       <c r="B485" t="s">
-        <v>242</v>
+        <v>170</v>
       </c>
       <c r="C485" t="s">
         <v>439</v>
@@ -7592,7 +7585,7 @@
         <v>5</v>
       </c>
       <c r="B486" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C486" t="s">
         <v>439</v>
@@ -7603,7 +7596,7 @@
         <v>5</v>
       </c>
       <c r="B487" t="s">
-        <v>187</v>
+        <v>243</v>
       </c>
       <c r="C487" t="s">
         <v>439</v>
@@ -7614,7 +7607,7 @@
         <v>5</v>
       </c>
       <c r="B488" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C488" t="s">
         <v>439</v>
@@ -7625,7 +7618,7 @@
         <v>5</v>
       </c>
       <c r="B489" t="s">
-        <v>521</v>
+        <v>188</v>
       </c>
       <c r="C489" t="s">
         <v>439</v>
@@ -7636,7 +7629,7 @@
         <v>5</v>
       </c>
       <c r="B490" t="s">
-        <v>191</v>
+        <v>521</v>
       </c>
       <c r="C490" t="s">
         <v>439</v>
@@ -7647,7 +7640,7 @@
         <v>5</v>
       </c>
       <c r="B491" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="C491" t="s">
         <v>439</v>
@@ -7658,18 +7651,29 @@
         <v>5</v>
       </c>
       <c r="B492" t="s">
+        <v>212</v>
+      </c>
+      <c r="C492" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="493" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A493" t="s">
+        <v>5</v>
+      </c>
+      <c r="B493" t="s">
         <v>213</v>
       </c>
-      <c r="C492" t="s">
+      <c r="C493" t="s">
         <v>439</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" autoFilter="0"/>
-  <autoFilter ref="A1:C492" xr:uid="{FA20B5A7-A3E2-3F42-944A-67FC92CE6A4B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C950">
-    <sortCondition ref="A2:A950"/>
-    <sortCondition ref="B2:B950"/>
+  <autoFilter ref="A1:C493" xr:uid="{FA20B5A7-A3E2-3F42-944A-67FC92CE6A4B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C951">
+    <sortCondition ref="A2:A951"/>
+    <sortCondition ref="B2:B951"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>